<commit_message>
Regression Daten und mehr
</commit_message>
<xml_diff>
--- a/data/Feiertage.xlsx
+++ b/data/Feiertage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tokes\Documents\GitHub\sca_case_study\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\TUB Master\1. Semester\SCA\Case study\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{361EA8F6-8A64-4210-8CFD-3580FFB6BE16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7D3344-A59C-43B3-AB84-56680868D63F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43065" yWindow="2040" windowWidth="3870" windowHeight="750" xr2:uid="{3D19F70E-A801-4AA0-B791-6182454455DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3D19F70E-A801-4AA0-B791-6182454455DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="159">
   <si>
     <t>CalenderWeek</t>
   </si>
@@ -508,6 +508,9 @@
   </si>
   <si>
     <t>2020-52</t>
+  </si>
+  <si>
+    <t>2020-53</t>
   </si>
 </sst>
 </file>
@@ -865,19 +868,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8988548-C848-449A-850F-E5DC7014DC0A}">
-  <dimension ref="A1:B157"/>
+  <dimension ref="A1:B158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="A158" sqref="A158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -885,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -893,7 +896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -901,7 +904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -909,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -917,7 +920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -925,7 +928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -933,7 +936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -941,7 +944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -949,7 +952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -957,7 +960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -965,7 +968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -973,7 +976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -981,7 +984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -989,7 +992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1005,7 +1008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1013,7 +1016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1021,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1029,7 +1032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1037,7 +1040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1045,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1053,7 +1056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1069,7 +1072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1077,7 +1080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1085,7 +1088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1093,7 +1096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1109,7 +1112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1117,7 +1120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1125,7 +1128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1133,7 +1136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1141,7 +1144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1149,7 +1152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1157,7 +1160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1165,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1181,7 +1184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1189,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1197,7 +1200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1205,7 +1208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1213,7 +1216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1221,7 +1224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1229,7 +1232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1237,7 +1240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1245,7 +1248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1253,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1269,7 +1272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1277,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -1285,7 +1288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1293,7 +1296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -1301,7 +1304,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -1309,7 +1312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -1317,7 +1320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -1325,7 +1328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -1333,7 +1336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -1357,7 +1360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -1365,7 +1368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -1373,7 +1376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -1381,7 +1384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -1389,7 +1392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -1405,7 +1408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -1413,7 +1416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -1421,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -1429,7 +1432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -1437,7 +1440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -1445,7 +1448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -1461,7 +1464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -1469,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -1477,7 +1480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -1485,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -1493,7 +1496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -1501,7 +1504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -1517,7 +1520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -1525,7 +1528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -1533,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -1541,7 +1544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>85</v>
       </c>
@@ -1557,7 +1560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>86</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -1573,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -1581,7 +1584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -1589,7 +1592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>90</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>91</v>
       </c>
@@ -1605,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>92</v>
       </c>
@@ -1613,7 +1616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>94</v>
       </c>
@@ -1629,7 +1632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>95</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>96</v>
       </c>
@@ -1645,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>97</v>
       </c>
@@ -1653,7 +1656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>98</v>
       </c>
@@ -1661,7 +1664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>99</v>
       </c>
@@ -1669,7 +1672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>100</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>101</v>
       </c>
@@ -1685,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>102</v>
       </c>
@@ -1693,7 +1696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>103</v>
       </c>
@@ -1701,7 +1704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>104</v>
       </c>
@@ -1709,7 +1712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>105</v>
       </c>
@@ -1717,7 +1720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>106</v>
       </c>
@@ -1725,7 +1728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>107</v>
       </c>
@@ -1733,7 +1736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>108</v>
       </c>
@@ -1741,7 +1744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>109</v>
       </c>
@@ -1749,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>110</v>
       </c>
@@ -1757,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>111</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>112</v>
       </c>
@@ -1773,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>113</v>
       </c>
@@ -1781,7 +1784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>114</v>
       </c>
@@ -1789,7 +1792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>115</v>
       </c>
@@ -1797,7 +1800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>116</v>
       </c>
@@ -1805,7 +1808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>117</v>
       </c>
@@ -1813,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>118</v>
       </c>
@@ -1821,7 +1824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>119</v>
       </c>
@@ -1829,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>120</v>
       </c>
@@ -1837,7 +1840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>121</v>
       </c>
@@ -1845,7 +1848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>122</v>
       </c>
@@ -1853,7 +1856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>123</v>
       </c>
@@ -1861,7 +1864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>124</v>
       </c>
@@ -1869,7 +1872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>125</v>
       </c>
@@ -1877,7 +1880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>126</v>
       </c>
@@ -1885,7 +1888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>127</v>
       </c>
@@ -1893,7 +1896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>128</v>
       </c>
@@ -1901,7 +1904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>129</v>
       </c>
@@ -1909,7 +1912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>130</v>
       </c>
@@ -1917,7 +1920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>131</v>
       </c>
@@ -1925,7 +1928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>132</v>
       </c>
@@ -1933,7 +1936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>133</v>
       </c>
@@ -1941,7 +1944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>134</v>
       </c>
@@ -1949,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>135</v>
       </c>
@@ -1957,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>136</v>
       </c>
@@ -1965,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>137</v>
       </c>
@@ -1973,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>138</v>
       </c>
@@ -1981,7 +1984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>139</v>
       </c>
@@ -1989,7 +1992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>140</v>
       </c>
@@ -1997,7 +2000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>141</v>
       </c>
@@ -2005,7 +2008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>142</v>
       </c>
@@ -2013,7 +2016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>143</v>
       </c>
@@ -2021,7 +2024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>144</v>
       </c>
@@ -2029,7 +2032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>145</v>
       </c>
@@ -2037,7 +2040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>146</v>
       </c>
@@ -2045,7 +2048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>147</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>148</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>149</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>150</v>
       </c>
@@ -2077,7 +2080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>151</v>
       </c>
@@ -2085,7 +2088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>152</v>
       </c>
@@ -2093,7 +2096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>153</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>154</v>
       </c>
@@ -2109,7 +2112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>155</v>
       </c>
@@ -2117,7 +2120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>156</v>
       </c>
@@ -2125,12 +2128,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>157</v>
       </c>
       <c r="B157">
         <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>158</v>
+      </c>
+      <c r="B158">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>